<commit_message>
add : resume for 2019
</commit_message>
<xml_diff>
--- a/2019 秋季招聘.xlsx
+++ b/2019 秋季招聘.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="秋招进度" sheetId="1" r:id="rId1"/>
-    <sheet name="TODO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>投递公司</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,27 +69,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>阿里</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>网易</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>阿里</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Need2do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完善秋招简历</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>复习简历内容</t>
+    <t>网申截止时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.8.17</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -114,7 +105,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
@@ -424,73 +415,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="9.75" customWidth="1"/>
-    <col min="7" max="7" width="15.75" customWidth="1"/>
-    <col min="8" max="9" width="14.25" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="21.75" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="9.75" customWidth="1"/>
+    <col min="8" max="8" width="15.75" customWidth="1"/>
+    <col min="9" max="10" width="14.25" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -498,43 +496,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="54.5" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>